<commit_message>
generate player list logic
</commit_message>
<xml_diff>
--- a/lista.xlsx
+++ b/lista.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -19,25 +19,64 @@
     <t>Nombre</t>
   </si>
   <si>
-    <t>Confirmo</t>
+    <t>Posición</t>
+  </si>
+  <si>
+    <t>David Alzate</t>
+  </si>
+  <si>
+    <t>Defensa Lateral</t>
   </si>
   <si>
     <t>Ricardo Martinez</t>
   </si>
   <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>David Alzate</t>
-  </si>
-  <si>
-    <t>Marcel</t>
-  </si>
-  <si>
-    <t>Luis Carlos</t>
-  </si>
-  <si>
-    <t>No</t>
+    <t>Volante Ofensivo</t>
+  </si>
+  <si>
+    <t>Santiago Martinez</t>
+  </si>
+  <si>
+    <t>Arquero</t>
+  </si>
+  <si>
+    <t>Marcel Sandoval</t>
+  </si>
+  <si>
+    <t>Defensa Central</t>
+  </si>
+  <si>
+    <t>Yeison Meza</t>
+  </si>
+  <si>
+    <t>William Valencia</t>
+  </si>
+  <si>
+    <t>Delantero</t>
+  </si>
+  <si>
+    <t>Angel Correa</t>
+  </si>
+  <si>
+    <t>Juan Herrera</t>
+  </si>
+  <si>
+    <t>Jhoan Zúñiga</t>
+  </si>
+  <si>
+    <t>Jhon Parra</t>
+  </si>
+  <si>
+    <t>Volante de Marca</t>
+  </si>
+  <si>
+    <t>Carlos Ruales</t>
+  </si>
+  <si>
+    <t>Sebastian Campos</t>
+  </si>
+  <si>
+    <t>Camilo Moncada</t>
   </si>
 </sst>
 </file>
@@ -47,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -58,6 +97,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -74,15 +117,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -311,7 +360,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -319,48 +368,213 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
-        <v>45490.52411402778</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="3">
+        <v>45493.41833877315</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
-        <v>45490.52423924769</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="3">
+        <v>45493.41846320602</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3">
+        <v>45493.4186741088</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>45493.41888982639</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>45493.41901109954</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>45493.41912380787</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>45493.41996944444</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3">
+        <v>45493.42009484954</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2">
-        <v>45490.52443027778</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="10">
+      <c r="A10" s="3">
+        <v>45493.42069460648</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2">
-        <v>45490.57776032407</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3">
+        <v>45493.431116377316</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3">
+        <v>45493.43122983797</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3">
+        <v>45493.43145978009</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3">
+        <v>45493.43167372685</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="5"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="5"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="5"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="5"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="5"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="5"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="5"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="5"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="5"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="5"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="5"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="5"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="5"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="5"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="5"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="5"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="5"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="5"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="5"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="5"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>